<commit_message>
Uploading updated excel and csv files
</commit_message>
<xml_diff>
--- a/Ghana.plants.uses.category.new.xlsx
+++ b/Ghana.plants.uses.category.new.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saray\Sarah\MASTERS PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saray\Sarah\MASTERS PROJECT\GhanaEcoServices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0B15E5F3-C231-4825-9D3B-9121DEB62AB8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4CFA2501-CE02-43CE-8D85-97048915785B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11521" uniqueCount="1609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11518" uniqueCount="1606">
   <si>
     <t>Species</t>
   </si>
@@ -5803,15 +5803,6 @@
   <si>
     <t>Cochlospermum 
 tinctorium A. Rich.</t>
-  </si>
-  <si>
-    <t>break the health care down</t>
-  </si>
-  <si>
-    <t>count the number of records</t>
-  </si>
-  <si>
-    <t>how many of the species have records in gbif</t>
   </si>
   <si>
     <t>Adiantum veneris</t>
@@ -7469,8 +7460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1039"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="C1022" workbookViewId="0">
+      <selection activeCell="D1035" sqref="D1035"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5"/>
@@ -7762,7 +7753,7 @@
         <v>174</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1">
@@ -7904,10 +7895,10 @@
         <v>265</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>266</v>
@@ -7952,10 +7943,10 @@
         <v>265</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>266</v>
@@ -7997,10 +7988,10 @@
         <v>147</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>148</v>
@@ -8300,10 +8291,10 @@
     </row>
     <row r="18" spans="1:16" ht="46.5">
       <c r="A18" s="2" t="s">
-        <v>1505</v>
+        <v>1502</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>1506</v>
+        <v>1503</v>
       </c>
       <c r="C18" s="29" t="s">
         <v>1450</v>
@@ -8327,10 +8318,10 @@
         <v>1090</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>1091</v>
@@ -8345,7 +8336,7 @@
         <v>452</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>1608</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -8377,10 +8368,10 @@
         <v>147</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>148</v>
@@ -9230,10 +9221,10 @@
         <v>147</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L37" s="5" t="s">
         <v>148</v>
@@ -9272,10 +9263,10 @@
         <v>1086</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>1087</v>
@@ -9290,7 +9281,7 @@
         <v>452</v>
       </c>
       <c r="P38" s="8" t="s">
-        <v>1507</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -9439,7 +9430,7 @@
     </row>
     <row r="42" spans="1:16" ht="21.5" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>1508</v>
+        <v>1505</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>201</v>
@@ -9466,7 +9457,7 @@
         <v>174</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1">
@@ -9602,10 +9593,10 @@
         <v>1086</v>
       </c>
       <c r="J45" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>1087</v>
@@ -9653,7 +9644,7 @@
         <v>72</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>49</v>
@@ -9701,7 +9692,7 @@
         <v>72</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>49</v>
@@ -9749,7 +9740,7 @@
         <v>72</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>49</v>
@@ -9881,10 +9872,10 @@
         <v>1086</v>
       </c>
       <c r="J51" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L51" s="5" t="s">
         <v>1087</v>
@@ -9923,10 +9914,10 @@
         <v>1086</v>
       </c>
       <c r="J52" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L52" s="5" t="s">
         <v>1087</v>
@@ -10307,7 +10298,7 @@
         <v>153</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K60" s="6" t="s">
         <v>154</v>
@@ -10403,10 +10394,10 @@
         <v>691</v>
       </c>
       <c r="J62" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L62" s="5" t="s">
         <v>692</v>
@@ -10499,7 +10490,7 @@
         <v>153</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K64" s="6" t="s">
         <v>154</v>
@@ -10547,10 +10538,10 @@
         <v>265</v>
       </c>
       <c r="J65" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K65" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L65" s="5" t="s">
         <v>266</v>
@@ -10595,10 +10586,10 @@
         <v>691</v>
       </c>
       <c r="J66" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K66" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L66" s="5" t="s">
         <v>692</v>
@@ -10787,7 +10778,7 @@
         <v>153</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K70" s="6" t="s">
         <v>154</v>
@@ -10835,7 +10826,7 @@
         <v>174</v>
       </c>
       <c r="J71" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K71" s="1"/>
       <c r="L71" s="1">
@@ -10881,7 +10872,7 @@
         <v>174</v>
       </c>
       <c r="J72" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K72" s="1"/>
       <c r="L72" s="1">
@@ -10927,7 +10918,7 @@
         <v>174</v>
       </c>
       <c r="J73" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K73" s="1"/>
       <c r="L73" s="1">
@@ -11021,10 +11012,10 @@
         <v>691</v>
       </c>
       <c r="J75" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L75" s="5" t="s">
         <v>692</v>
@@ -11165,10 +11156,10 @@
         <v>1382</v>
       </c>
       <c r="J78" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K78" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L78" s="5" t="s">
         <v>1414</v>
@@ -11216,7 +11207,7 @@
         <v>72</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L79" s="5" t="s">
         <v>49</v>
@@ -11405,7 +11396,7 @@
         <v>174</v>
       </c>
       <c r="J83" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K83" s="1"/>
       <c r="L83" s="1">
@@ -11493,10 +11484,10 @@
         <v>1086</v>
       </c>
       <c r="J85" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L85" s="5" t="s">
         <v>1087</v>
@@ -11589,7 +11580,7 @@
         <v>174</v>
       </c>
       <c r="J87" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K87" s="1"/>
       <c r="L87" s="1">
@@ -11779,10 +11770,10 @@
         <v>1382</v>
       </c>
       <c r="J91" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K91" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L91" s="5" t="s">
         <v>1410</v>
@@ -12067,10 +12058,10 @@
         <v>1382</v>
       </c>
       <c r="J97" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K97" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L97" s="5" t="s">
         <v>1419</v>
@@ -12259,7 +12250,7 @@
         <v>174</v>
       </c>
       <c r="J101" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K101" s="1"/>
       <c r="L101" s="1">
@@ -12305,10 +12296,10 @@
         <v>1382</v>
       </c>
       <c r="J102" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K102" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L102" s="5" t="s">
         <v>1412</v>
@@ -12353,7 +12344,7 @@
         <v>153</v>
       </c>
       <c r="J103" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K103" s="6" t="s">
         <v>154</v>
@@ -12689,10 +12680,10 @@
         <v>265</v>
       </c>
       <c r="J110" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K110" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L110" s="5" t="s">
         <v>266</v>
@@ -12785,10 +12776,10 @@
         <v>147</v>
       </c>
       <c r="J112" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K112" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L112" s="5" t="s">
         <v>148</v>
@@ -12833,10 +12824,10 @@
         <v>1090</v>
       </c>
       <c r="J113" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K113" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L113" s="5" t="s">
         <v>1091</v>
@@ -13019,10 +13010,10 @@
         <v>1086</v>
       </c>
       <c r="J117" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K117" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L117" s="5" t="s">
         <v>1087</v>
@@ -13461,7 +13452,7 @@
     </row>
     <row r="127" spans="1:16">
       <c r="A127" s="12" t="s">
-        <v>1509</v>
+        <v>1506</v>
       </c>
       <c r="B127" s="12" t="s">
         <v>270</v>
@@ -13488,10 +13479,10 @@
         <v>265</v>
       </c>
       <c r="J127" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K127" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L127" s="5" t="s">
         <v>266</v>
@@ -13509,7 +13500,7 @@
     </row>
     <row r="128" spans="1:16">
       <c r="A128" s="12" t="s">
-        <v>1509</v>
+        <v>1506</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>270</v>
@@ -13536,10 +13527,10 @@
         <v>265</v>
       </c>
       <c r="J128" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K128" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L128" s="5" t="s">
         <v>266</v>
@@ -13872,7 +13863,7 @@
         <v>153</v>
       </c>
       <c r="J135" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K135" s="6" t="s">
         <v>154</v>
@@ -13920,7 +13911,7 @@
         <v>174</v>
       </c>
       <c r="J136" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K136" s="1"/>
       <c r="L136" s="1">
@@ -13966,10 +13957,10 @@
         <v>1090</v>
       </c>
       <c r="J137" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K137" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L137" s="5" t="s">
         <v>1091</v>
@@ -14014,10 +14005,10 @@
         <v>147</v>
       </c>
       <c r="J138" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K138" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L138" s="5" t="s">
         <v>148</v>
@@ -14158,10 +14149,10 @@
         <v>1382</v>
       </c>
       <c r="J141" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K141" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L141" s="5" t="s">
         <v>1432</v>
@@ -14299,10 +14290,10 @@
         <v>688</v>
       </c>
       <c r="J144" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K144" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L144" s="5" t="s">
         <v>689</v>
@@ -14347,10 +14338,10 @@
         <v>691</v>
       </c>
       <c r="J145" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K145" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L145" s="5" t="s">
         <v>692</v>
@@ -14672,7 +14663,7 @@
         <v>72</v>
       </c>
       <c r="K152" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L152" s="5" t="s">
         <v>49</v>
@@ -14765,10 +14756,10 @@
         <v>1382</v>
       </c>
       <c r="J154" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K154" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L154" s="5" t="s">
         <v>1434</v>
@@ -14957,7 +14948,7 @@
         <v>174</v>
       </c>
       <c r="J158" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K158" s="1"/>
       <c r="L158" s="1">
@@ -15192,7 +15183,7 @@
         <v>174</v>
       </c>
       <c r="J163" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K163" s="1"/>
       <c r="L163" s="1">
@@ -15235,7 +15226,7 @@
         <v>174</v>
       </c>
       <c r="J164" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K164" s="1"/>
       <c r="L164" s="1">
@@ -15278,7 +15269,7 @@
         <v>174</v>
       </c>
       <c r="J165" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K165" s="1"/>
       <c r="L165" s="1">
@@ -15420,10 +15411,10 @@
         <v>691</v>
       </c>
       <c r="J168" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K168" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L168" s="5" t="s">
         <v>692</v>
@@ -15489,7 +15480,7 @@
     </row>
     <row r="170" spans="1:16">
       <c r="A170" s="2" t="s">
-        <v>1510</v>
+        <v>1507</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>273</v>
@@ -15516,10 +15507,10 @@
         <v>265</v>
       </c>
       <c r="J170" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K170" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L170" s="5" t="s">
         <v>266</v>
@@ -15804,7 +15795,7 @@
         <v>153</v>
       </c>
       <c r="J176" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K176" s="6" t="s">
         <v>154</v>
@@ -15852,7 +15843,7 @@
         <v>174</v>
       </c>
       <c r="J177" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K177" s="1"/>
       <c r="L177" s="1">
@@ -15898,7 +15889,7 @@
         <v>174</v>
       </c>
       <c r="J178" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K178" s="1"/>
       <c r="L178" s="1">
@@ -16130,10 +16121,10 @@
         <v>1086</v>
       </c>
       <c r="J183" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K183" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L183" s="5" t="s">
         <v>1087</v>
@@ -16151,7 +16142,7 @@
     </row>
     <row r="184" spans="1:16">
       <c r="A184" s="2" t="s">
-        <v>1511</v>
+        <v>1508</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>274</v>
@@ -16178,10 +16169,10 @@
         <v>265</v>
       </c>
       <c r="J184" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K184" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L184" s="5" t="s">
         <v>266</v>
@@ -16199,7 +16190,7 @@
     </row>
     <row r="185" spans="1:16" ht="31">
       <c r="A185" s="2" t="s">
-        <v>1512</v>
+        <v>1509</v>
       </c>
       <c r="B185" s="30" t="s">
         <v>1035</v>
@@ -16274,7 +16265,7 @@
         <v>174</v>
       </c>
       <c r="J186" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K186" s="1"/>
       <c r="L186" s="1">
@@ -16368,10 +16359,10 @@
         <v>1090</v>
       </c>
       <c r="J188" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K188" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L188" s="5" t="s">
         <v>1091</v>
@@ -16416,7 +16407,7 @@
         <v>153</v>
       </c>
       <c r="J189" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K189" s="6" t="s">
         <v>154</v>
@@ -16629,7 +16620,7 @@
     </row>
     <row r="194" spans="1:16" ht="31">
       <c r="A194" s="11" t="s">
-        <v>1513</v>
+        <v>1510</v>
       </c>
       <c r="B194" s="11" t="s">
         <v>935</v>
@@ -16906,7 +16897,7 @@
     </row>
     <row r="200" spans="1:16" ht="31">
       <c r="A200" s="2" t="s">
-        <v>1514</v>
+        <v>1511</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>179</v>
@@ -16933,7 +16924,7 @@
         <v>174</v>
       </c>
       <c r="J200" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K200" s="1"/>
       <c r="L200" s="1">
@@ -16952,7 +16943,7 @@
     </row>
     <row r="201" spans="1:16">
       <c r="A201" s="10" t="s">
-        <v>1515</v>
+        <v>1512</v>
       </c>
       <c r="B201" s="10" t="s">
         <v>1475</v>
@@ -16979,10 +16970,10 @@
         <v>265</v>
       </c>
       <c r="J201" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K201" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L201" s="5" t="s">
         <v>266</v>
@@ -17000,7 +16991,7 @@
     </row>
     <row r="202" spans="1:16" ht="31">
       <c r="A202" s="2" t="s">
-        <v>1515</v>
+        <v>1512</v>
       </c>
       <c r="B202" s="24" t="s">
         <v>1474</v>
@@ -17072,10 +17063,10 @@
         <v>688</v>
       </c>
       <c r="J203" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K203" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L203" s="5" t="s">
         <v>689</v>
@@ -17637,10 +17628,10 @@
         <v>147</v>
       </c>
       <c r="J215" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K215" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L215" s="5" t="s">
         <v>148</v>
@@ -17685,7 +17676,7 @@
         <v>153</v>
       </c>
       <c r="J216" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K216" s="6" t="s">
         <v>154</v>
@@ -17829,10 +17820,10 @@
         <v>1382</v>
       </c>
       <c r="J219" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K219" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L219" s="5" t="s">
         <v>1420</v>
@@ -18099,7 +18090,7 @@
         <v>1450</v>
       </c>
       <c r="D225" s="7" t="s">
-        <v>1596</v>
+        <v>1593</v>
       </c>
       <c r="E225" s="1" t="s">
         <v>1134</v>
@@ -18120,7 +18111,7 @@
         <v>72</v>
       </c>
       <c r="K225" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L225" s="5" t="s">
         <v>49</v>
@@ -18165,7 +18156,7 @@
         <v>174</v>
       </c>
       <c r="J226" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K226" s="1"/>
       <c r="L226" s="1">
@@ -18211,7 +18202,7 @@
         <v>174</v>
       </c>
       <c r="J227" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K227" s="1"/>
       <c r="L227" s="1">
@@ -18251,10 +18242,10 @@
         <v>1086</v>
       </c>
       <c r="J228" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K228" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L228" s="5" t="s">
         <v>1087</v>
@@ -18320,7 +18311,7 @@
     </row>
     <row r="230" spans="1:16">
       <c r="A230" s="2" t="s">
-        <v>1516</v>
+        <v>1513</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>276</v>
@@ -18347,10 +18338,10 @@
         <v>265</v>
       </c>
       <c r="J230" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K230" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L230" s="5" t="s">
         <v>266</v>
@@ -18398,7 +18389,7 @@
         <v>72</v>
       </c>
       <c r="K231" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L231" s="5" t="s">
         <v>49</v>
@@ -18446,7 +18437,7 @@
         <v>72</v>
       </c>
       <c r="K232" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L232" s="5" t="s">
         <v>49</v>
@@ -18539,7 +18530,7 @@
         <v>72</v>
       </c>
       <c r="K234" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L234" s="5" t="s">
         <v>49</v>
@@ -18587,7 +18578,7 @@
         <v>72</v>
       </c>
       <c r="K235" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L235" s="5" t="s">
         <v>49</v>
@@ -18632,10 +18623,10 @@
         <v>147</v>
       </c>
       <c r="J236" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K236" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L236" s="5" t="s">
         <v>148</v>
@@ -18866,10 +18857,10 @@
         <v>688</v>
       </c>
       <c r="J241" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K241" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L241" s="5" t="s">
         <v>689</v>
@@ -18914,10 +18905,10 @@
         <v>265</v>
       </c>
       <c r="J242" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K242" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L242" s="5" t="s">
         <v>266</v>
@@ -18983,7 +18974,7 @@
     </row>
     <row r="244" spans="1:16">
       <c r="A244" s="2" t="s">
-        <v>1517</v>
+        <v>1514</v>
       </c>
       <c r="C244" s="29" t="s">
         <v>1449</v>
@@ -19047,10 +19038,10 @@
         <v>265</v>
       </c>
       <c r="J245" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K245" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L245" s="5" t="s">
         <v>266</v>
@@ -19377,10 +19368,10 @@
         <v>688</v>
       </c>
       <c r="J252" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K252" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L252" s="5" t="s">
         <v>689</v>
@@ -19428,7 +19419,7 @@
         <v>72</v>
       </c>
       <c r="K253" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L253" s="5" t="s">
         <v>49</v>
@@ -19476,7 +19467,7 @@
         <v>72</v>
       </c>
       <c r="K254" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L254" s="5" t="s">
         <v>49</v>
@@ -19521,10 +19512,10 @@
         <v>691</v>
       </c>
       <c r="J255" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K255" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L255" s="5" t="s">
         <v>692</v>
@@ -19617,10 +19608,10 @@
         <v>1382</v>
       </c>
       <c r="J257" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K257" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L257" s="5" t="s">
         <v>1416</v>
@@ -19840,10 +19831,10 @@
         <v>1086</v>
       </c>
       <c r="J262" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K262" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L262" s="5" t="s">
         <v>1087</v>
@@ -19882,10 +19873,10 @@
         <v>1086</v>
       </c>
       <c r="J263" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K263" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L263" s="5" t="s">
         <v>1087</v>
@@ -19924,10 +19915,10 @@
         <v>1181</v>
       </c>
       <c r="J264" s="23" t="s">
-        <v>1597</v>
+        <v>1594</v>
       </c>
       <c r="K264" s="6" t="s">
-        <v>1598</v>
+        <v>1595</v>
       </c>
       <c r="L264" s="5" t="s">
         <v>1182</v>
@@ -19972,7 +19963,7 @@
         <v>174</v>
       </c>
       <c r="J265" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K265" s="1"/>
       <c r="L265" s="1">
@@ -20018,7 +20009,7 @@
         <v>174</v>
       </c>
       <c r="J266" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K266" s="1"/>
       <c r="L266" s="1">
@@ -20626,10 +20617,10 @@
         <v>688</v>
       </c>
       <c r="J279" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K279" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L279" s="5" t="s">
         <v>689</v>
@@ -20674,7 +20665,7 @@
         <v>174</v>
       </c>
       <c r="J280" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K280" s="1"/>
       <c r="L280" s="1">
@@ -20778,7 +20769,7 @@
     </row>
     <row r="283" spans="1:16">
       <c r="A283" s="2" t="s">
-        <v>1518</v>
+        <v>1515</v>
       </c>
       <c r="C283" s="29" t="s">
         <v>1449</v>
@@ -20815,7 +20806,7 @@
     </row>
     <row r="284" spans="1:16">
       <c r="A284" s="2" t="s">
-        <v>1518</v>
+        <v>1515</v>
       </c>
       <c r="B284" s="11" t="s">
         <v>258</v>
@@ -20863,7 +20854,7 @@
     </row>
     <row r="285" spans="1:16">
       <c r="A285" s="2" t="s">
-        <v>1518</v>
+        <v>1515</v>
       </c>
       <c r="B285" s="11" t="s">
         <v>258</v>
@@ -20911,7 +20902,7 @@
     </row>
     <row r="286" spans="1:16">
       <c r="A286" s="2" t="s">
-        <v>1518</v>
+        <v>1515</v>
       </c>
       <c r="B286" s="18" t="s">
         <v>662</v>
@@ -20959,7 +20950,7 @@
     </row>
     <row r="287" spans="1:16">
       <c r="A287" s="2" t="s">
-        <v>1518</v>
+        <v>1515</v>
       </c>
       <c r="B287" s="24" t="s">
         <v>1386</v>
@@ -20986,10 +20977,10 @@
         <v>1382</v>
       </c>
       <c r="J287" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K287" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L287" s="5" t="s">
         <v>1413</v>
@@ -21007,7 +20998,7 @@
     </row>
     <row r="288" spans="1:16">
       <c r="A288" s="2" t="s">
-        <v>1518</v>
+        <v>1515</v>
       </c>
       <c r="B288" s="19" t="s">
         <v>721</v>
@@ -21172,10 +21163,10 @@
         <v>1086</v>
       </c>
       <c r="J291" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K291" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L291" s="5" t="s">
         <v>1087</v>
@@ -21316,10 +21307,10 @@
         <v>147</v>
       </c>
       <c r="J294" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K294" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L294" s="5" t="s">
         <v>148</v>
@@ -21337,7 +21328,7 @@
     </row>
     <row r="295" spans="1:16">
       <c r="A295" s="30" t="s">
-        <v>1519</v>
+        <v>1516</v>
       </c>
       <c r="B295" s="30" t="s">
         <v>1501</v>
@@ -21385,7 +21376,7 @@
     </row>
     <row r="296" spans="1:16">
       <c r="A296" s="30" t="s">
-        <v>1519</v>
+        <v>1516</v>
       </c>
       <c r="B296" s="30" t="s">
         <v>1501</v>
@@ -21460,10 +21451,10 @@
         <v>265</v>
       </c>
       <c r="J297" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K297" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L297" s="5" t="s">
         <v>266</v>
@@ -21556,10 +21547,10 @@
         <v>691</v>
       </c>
       <c r="J299" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K299" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L299" s="5" t="s">
         <v>692</v>
@@ -21662,7 +21653,7 @@
     </row>
     <row r="302" spans="1:16">
       <c r="A302" s="11" t="s">
-        <v>1520</v>
+        <v>1517</v>
       </c>
       <c r="B302" s="11" t="s">
         <v>701</v>
@@ -21689,10 +21680,10 @@
         <v>691</v>
       </c>
       <c r="J302" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K302" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L302" s="5" t="s">
         <v>692</v>
@@ -22025,10 +22016,10 @@
         <v>1090</v>
       </c>
       <c r="J309" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K309" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L309" s="5" t="s">
         <v>1091</v>
@@ -22313,10 +22304,10 @@
         <v>147</v>
       </c>
       <c r="J315" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K315" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L315" s="5" t="s">
         <v>148</v>
@@ -22364,7 +22355,7 @@
         <v>72</v>
       </c>
       <c r="K316" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L316" s="5" t="s">
         <v>49</v>
@@ -22412,7 +22403,7 @@
         <v>72</v>
       </c>
       <c r="K317" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L317" s="5" t="s">
         <v>49</v>
@@ -22505,10 +22496,10 @@
         <v>265</v>
       </c>
       <c r="J319" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K319" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L319" s="5" t="s">
         <v>266</v>
@@ -22526,7 +22517,7 @@
     </row>
     <row r="320" spans="1:16">
       <c r="A320" s="19" t="s">
-        <v>1521</v>
+        <v>1518</v>
       </c>
       <c r="B320" s="19" t="s">
         <v>738</v>
@@ -22574,7 +22565,7 @@
     </row>
     <row r="321" spans="1:16" ht="31">
       <c r="A321" s="11" t="s">
-        <v>1522</v>
+        <v>1519</v>
       </c>
       <c r="B321" s="11" t="s">
         <v>893</v>
@@ -22622,7 +22613,7 @@
     </row>
     <row r="322" spans="1:16" ht="31">
       <c r="A322" s="11" t="s">
-        <v>1523</v>
+        <v>1520</v>
       </c>
       <c r="B322" s="11" t="s">
         <v>894</v>
@@ -22715,7 +22706,7 @@
     </row>
     <row r="324" spans="1:16" ht="31">
       <c r="A324" s="11" t="s">
-        <v>1524</v>
+        <v>1521</v>
       </c>
       <c r="B324" s="11" t="s">
         <v>886</v>
@@ -22790,7 +22781,7 @@
         <v>174</v>
       </c>
       <c r="J325" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K325" s="1"/>
       <c r="L325" s="1">
@@ -22836,7 +22827,7 @@
         <v>174</v>
       </c>
       <c r="J326" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K326" s="1"/>
       <c r="L326" s="1">
@@ -22882,7 +22873,7 @@
         <v>131</v>
       </c>
       <c r="J327" s="23" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="K327" s="1" t="s">
         <v>130</v>
@@ -22930,7 +22921,7 @@
         <v>131</v>
       </c>
       <c r="J328" s="23" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="K328" s="1" t="s">
         <v>130</v>
@@ -22978,7 +22969,7 @@
         <v>131</v>
       </c>
       <c r="J329" s="23" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="K329" s="1" t="s">
         <v>130</v>
@@ -23026,7 +23017,7 @@
         <v>131</v>
       </c>
       <c r="J330" s="23" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="K330" s="1" t="s">
         <v>130</v>
@@ -23074,10 +23065,10 @@
         <v>1090</v>
       </c>
       <c r="J331" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K331" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L331" s="5" t="s">
         <v>1091</v>
@@ -23317,7 +23308,7 @@
         <v>72</v>
       </c>
       <c r="K336" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L336" s="5" t="s">
         <v>49</v>
@@ -23365,7 +23356,7 @@
         <v>72</v>
       </c>
       <c r="K337" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L337" s="5" t="s">
         <v>49</v>
@@ -23383,7 +23374,7 @@
     </row>
     <row r="338" spans="1:16">
       <c r="A338" s="2" t="s">
-        <v>1525</v>
+        <v>1522</v>
       </c>
       <c r="B338" s="2" t="s">
         <v>1111</v>
@@ -23410,10 +23401,10 @@
         <v>1090</v>
       </c>
       <c r="J338" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K338" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L338" s="5" t="s">
         <v>1091</v>
@@ -23465,7 +23456,7 @@
         <v>452</v>
       </c>
       <c r="P339" s="8" t="s">
-        <v>1526</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="340" spans="1:16">
@@ -23689,10 +23680,10 @@
         <v>265</v>
       </c>
       <c r="J344" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K344" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L344" s="5" t="s">
         <v>266</v>
@@ -23788,7 +23779,7 @@
         <v>72</v>
       </c>
       <c r="K346" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L346" s="5" t="s">
         <v>49</v>
@@ -23899,7 +23890,7 @@
     </row>
     <row r="349" spans="1:16" ht="31">
       <c r="A349" s="11" t="s">
-        <v>1527</v>
+        <v>1524</v>
       </c>
       <c r="B349" s="11" t="s">
         <v>900</v>
@@ -23995,7 +23986,7 @@
     </row>
     <row r="351" spans="1:16">
       <c r="A351" s="12" t="s">
-        <v>1528</v>
+        <v>1525</v>
       </c>
       <c r="B351" s="12" t="s">
         <v>281</v>
@@ -24022,10 +24013,10 @@
         <v>265</v>
       </c>
       <c r="J351" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K351" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L351" s="5" t="s">
         <v>266</v>
@@ -24043,7 +24034,7 @@
     </row>
     <row r="352" spans="1:16">
       <c r="A352" s="19" t="s">
-        <v>1529</v>
+        <v>1526</v>
       </c>
       <c r="B352" s="19" t="s">
         <v>719</v>
@@ -24166,10 +24157,10 @@
         <v>1382</v>
       </c>
       <c r="J354" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K354" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L354" s="5" t="s">
         <v>1435</v>
@@ -24331,7 +24322,7 @@
     </row>
     <row r="358" spans="1:16">
       <c r="A358" s="11" t="s">
-        <v>1530</v>
+        <v>1527</v>
       </c>
       <c r="B358" s="11" t="s">
         <v>705</v>
@@ -24358,10 +24349,10 @@
         <v>691</v>
       </c>
       <c r="J358" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K358" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L358" s="5" t="s">
         <v>692</v>
@@ -24403,10 +24394,10 @@
         <v>688</v>
       </c>
       <c r="J359" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K359" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L359" s="5" t="s">
         <v>689</v>
@@ -24424,7 +24415,7 @@
     </row>
     <row r="360" spans="1:16">
       <c r="A360" s="11" t="s">
-        <v>1531</v>
+        <v>1528</v>
       </c>
       <c r="B360" s="11" t="s">
         <v>706</v>
@@ -24451,10 +24442,10 @@
         <v>691</v>
       </c>
       <c r="J360" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K360" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L360" s="5" t="s">
         <v>692</v>
@@ -24499,7 +24490,7 @@
         <v>174</v>
       </c>
       <c r="J361" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K361" s="1"/>
       <c r="L361" s="1">
@@ -24518,7 +24509,7 @@
     </row>
     <row r="362" spans="1:16" ht="31">
       <c r="A362" s="11" t="s">
-        <v>1532</v>
+        <v>1529</v>
       </c>
       <c r="B362" s="11" t="s">
         <v>902</v>
@@ -24756,7 +24747,7 @@
     </row>
     <row r="367" spans="1:16">
       <c r="A367" s="2" t="s">
-        <v>1533</v>
+        <v>1530</v>
       </c>
       <c r="C367" s="29" t="s">
         <v>1449</v>
@@ -25315,7 +25306,7 @@
     </row>
     <row r="379" spans="1:16" ht="31">
       <c r="A379" s="11" t="s">
-        <v>1534</v>
+        <v>1531</v>
       </c>
       <c r="B379" s="11" t="s">
         <v>904</v>
@@ -25363,7 +25354,7 @@
     </row>
     <row r="380" spans="1:16" ht="31">
       <c r="A380" s="11" t="s">
-        <v>1535</v>
+        <v>1532</v>
       </c>
       <c r="B380" s="11" t="s">
         <v>905</v>
@@ -25408,7 +25399,7 @@
         <v>452</v>
       </c>
       <c r="P380" s="8" t="s">
-        <v>1536</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="381" spans="1:16" ht="31">
@@ -25458,7 +25449,7 @@
         <v>1989</v>
       </c>
       <c r="P381" s="8" t="s">
-        <v>1536</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="382" spans="1:16">
@@ -25586,10 +25577,10 @@
         <v>265</v>
       </c>
       <c r="J384" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K384" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L384" s="5" t="s">
         <v>266</v>
@@ -25970,7 +25961,7 @@
         <v>174</v>
       </c>
       <c r="J392" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K392" s="1"/>
       <c r="L392" s="1">
@@ -26016,7 +26007,7 @@
         <v>174</v>
       </c>
       <c r="J393" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K393" s="1"/>
       <c r="L393" s="1">
@@ -26062,10 +26053,10 @@
         <v>691</v>
       </c>
       <c r="J394" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K394" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L394" s="5" t="s">
         <v>692</v>
@@ -26158,7 +26149,7 @@
         <v>174</v>
       </c>
       <c r="J396" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K396" s="1"/>
       <c r="L396" s="1">
@@ -26177,7 +26168,7 @@
     </row>
     <row r="397" spans="1:16" ht="31">
       <c r="A397" s="2" t="s">
-        <v>1537</v>
+        <v>1534</v>
       </c>
       <c r="B397" s="2" t="s">
         <v>195</v>
@@ -26204,7 +26195,7 @@
         <v>174</v>
       </c>
       <c r="J397" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K397" s="1"/>
       <c r="L397" s="1">
@@ -26394,10 +26385,10 @@
         <v>1090</v>
       </c>
       <c r="J401" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K401" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L401" s="1" t="s">
         <v>1091</v>
@@ -26674,7 +26665,7 @@
         <v>72</v>
       </c>
       <c r="K407" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L407" s="5" t="s">
         <v>49</v>
@@ -27148,7 +27139,7 @@
         <v>174</v>
       </c>
       <c r="J417" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K417" s="1"/>
       <c r="L417" s="1">
@@ -27215,7 +27206,7 @@
     </row>
     <row r="419" spans="1:16" ht="31">
       <c r="A419" s="11" t="s">
-        <v>1538</v>
+        <v>1535</v>
       </c>
       <c r="B419" s="11" t="s">
         <v>928</v>
@@ -27290,7 +27281,7 @@
         <v>153</v>
       </c>
       <c r="J420" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K420" s="6" t="s">
         <v>154</v>
@@ -27530,10 +27521,10 @@
         <v>1174</v>
       </c>
       <c r="J425" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K425" s="6" t="s">
-        <v>1600</v>
+        <v>1597</v>
       </c>
       <c r="L425" s="5" t="s">
         <v>1175</v>
@@ -27764,10 +27755,10 @@
         <v>1086</v>
       </c>
       <c r="J430" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K430" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L430" s="5" t="s">
         <v>1087</v>
@@ -27956,10 +27947,10 @@
         <v>147</v>
       </c>
       <c r="J434" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K434" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L434" s="5" t="s">
         <v>148</v>
@@ -28052,10 +28043,10 @@
         <v>147</v>
       </c>
       <c r="J436" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K436" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L436" s="5" t="s">
         <v>148</v>
@@ -28196,10 +28187,10 @@
         <v>1382</v>
       </c>
       <c r="J439" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K439" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L439" s="5" t="s">
         <v>1415</v>
@@ -28343,7 +28334,7 @@
         <v>72</v>
       </c>
       <c r="K442" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L442" s="5" t="s">
         <v>49</v>
@@ -28391,7 +28382,7 @@
         <v>72</v>
       </c>
       <c r="K443" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L443" s="5" t="s">
         <v>49</v>
@@ -28439,7 +28430,7 @@
         <v>72</v>
       </c>
       <c r="K444" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L444" s="5" t="s">
         <v>49</v>
@@ -28484,7 +28475,7 @@
         <v>72</v>
       </c>
       <c r="K445" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L445" s="5" t="s">
         <v>54</v>
@@ -28529,10 +28520,10 @@
         <v>147</v>
       </c>
       <c r="J446" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K446" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L446" s="5" t="s">
         <v>148</v>
@@ -28553,7 +28544,7 @@
         <v>40</v>
       </c>
       <c r="B447" s="30" t="s">
-        <v>1539</v>
+        <v>1536</v>
       </c>
       <c r="C447" s="22" t="s">
         <v>1450</v>
@@ -28601,7 +28592,7 @@
         <v>40</v>
       </c>
       <c r="B448" s="30" t="s">
-        <v>1539</v>
+        <v>1536</v>
       </c>
       <c r="C448" s="22" t="s">
         <v>1451</v>
@@ -28913,10 +28904,10 @@
         <v>1174</v>
       </c>
       <c r="J454" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K454" s="6" t="s">
-        <v>1600</v>
+        <v>1597</v>
       </c>
       <c r="L454" s="5" t="s">
         <v>1175</v>
@@ -28955,10 +28946,10 @@
         <v>1086</v>
       </c>
       <c r="J455" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K455" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L455" s="5" t="s">
         <v>1087</v>
@@ -29003,7 +28994,7 @@
         <v>174</v>
       </c>
       <c r="J456" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K456" s="1"/>
       <c r="L456" s="1">
@@ -29049,7 +29040,7 @@
         <v>174</v>
       </c>
       <c r="J457" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K457" s="1"/>
       <c r="L457" s="1">
@@ -29095,10 +29086,10 @@
         <v>265</v>
       </c>
       <c r="J458" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K458" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L458" s="5" t="s">
         <v>266</v>
@@ -29489,7 +29480,7 @@
     </row>
     <row r="467" spans="1:16">
       <c r="A467" s="19" t="s">
-        <v>1540</v>
+        <v>1537</v>
       </c>
       <c r="B467" s="19" t="s">
         <v>733</v>
@@ -29660,10 +29651,10 @@
         <v>147</v>
       </c>
       <c r="J470" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K470" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L470" s="5" t="s">
         <v>148</v>
@@ -29708,10 +29699,10 @@
         <v>265</v>
       </c>
       <c r="J471" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K471" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L471" s="5" t="s">
         <v>266</v>
@@ -29759,7 +29750,7 @@
         <v>72</v>
       </c>
       <c r="K472" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L472" s="5" t="s">
         <v>49</v>
@@ -29852,10 +29843,10 @@
         <v>1090</v>
       </c>
       <c r="J474" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K474" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L474" s="5" t="s">
         <v>1091</v>
@@ -29900,7 +29891,7 @@
         <v>174</v>
       </c>
       <c r="J475" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K475" s="1"/>
       <c r="L475" s="1">
@@ -30285,7 +30276,7 @@
         <v>72</v>
       </c>
       <c r="K483" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L483" s="5" t="s">
         <v>49</v>
@@ -30330,10 +30321,10 @@
         <v>691</v>
       </c>
       <c r="J484" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K484" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L484" s="5" t="s">
         <v>692</v>
@@ -30474,10 +30465,10 @@
         <v>147</v>
       </c>
       <c r="J487" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K487" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L487" s="5" t="s">
         <v>148</v>
@@ -30570,10 +30561,10 @@
         <v>147</v>
       </c>
       <c r="J489" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K489" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L489" s="5" t="s">
         <v>148</v>
@@ -30618,10 +30609,10 @@
         <v>265</v>
       </c>
       <c r="J490" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K490" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L490" s="5" t="s">
         <v>266</v>
@@ -30666,10 +30657,10 @@
         <v>265</v>
       </c>
       <c r="J491" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K491" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L491" s="5" t="s">
         <v>266</v>
@@ -30810,10 +30801,10 @@
         <v>147</v>
       </c>
       <c r="J494" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K494" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L494" s="5" t="s">
         <v>148</v>
@@ -30858,7 +30849,7 @@
         <v>174</v>
       </c>
       <c r="J495" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K495" s="1"/>
       <c r="L495" s="1">
@@ -31024,7 +31015,7 @@
         <v>483</v>
       </c>
       <c r="B499" s="2" t="s">
-        <v>1542</v>
+        <v>1539</v>
       </c>
       <c r="C499" s="29" t="s">
         <v>1450</v>
@@ -31048,7 +31039,7 @@
         <v>174</v>
       </c>
       <c r="J499" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K499" s="1"/>
       <c r="L499" s="1">
@@ -31064,7 +31055,7 @@
         <v>452</v>
       </c>
       <c r="P499" s="8" t="s">
-        <v>1541</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="500" spans="1:16">
@@ -31144,10 +31135,10 @@
         <v>147</v>
       </c>
       <c r="J501" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K501" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L501" s="5" t="s">
         <v>148</v>
@@ -31213,7 +31204,7 @@
     </row>
     <row r="503" spans="1:16">
       <c r="A503" s="19" t="s">
-        <v>1543</v>
+        <v>1540</v>
       </c>
       <c r="B503" s="19" t="s">
         <v>717</v>
@@ -31336,10 +31327,10 @@
         <v>1090</v>
       </c>
       <c r="J505" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K505" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L505" s="5" t="s">
         <v>1091</v>
@@ -31384,10 +31375,10 @@
         <v>1382</v>
       </c>
       <c r="J506" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K506" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L506" s="5" t="s">
         <v>1383</v>
@@ -31405,7 +31396,7 @@
     </row>
     <row r="507" spans="1:16" ht="31">
       <c r="A507" s="11" t="s">
-        <v>1544</v>
+        <v>1541</v>
       </c>
       <c r="B507" s="11" t="s">
         <v>899</v>
@@ -31768,10 +31759,10 @@
         <v>265</v>
       </c>
       <c r="J514" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K514" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L514" s="5" t="s">
         <v>266</v>
@@ -31960,7 +31951,7 @@
         <v>174</v>
       </c>
       <c r="J518" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K518" s="1"/>
       <c r="L518" s="1">
@@ -32006,10 +31997,10 @@
         <v>147</v>
       </c>
       <c r="J519" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K519" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L519" s="5" t="s">
         <v>148</v>
@@ -32234,10 +32225,10 @@
         <v>688</v>
       </c>
       <c r="J524" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K524" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L524" s="5" t="s">
         <v>689</v>
@@ -32463,7 +32454,7 @@
         <v>174</v>
       </c>
       <c r="J529" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K529" s="1"/>
       <c r="L529" s="1">
@@ -32749,10 +32740,10 @@
         <v>147</v>
       </c>
       <c r="J535" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K535" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L535" s="5" t="s">
         <v>148</v>
@@ -32989,10 +32980,10 @@
         <v>1382</v>
       </c>
       <c r="J540" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K540" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L540" s="5" t="s">
         <v>1438</v>
@@ -33037,7 +33028,7 @@
         <v>174</v>
       </c>
       <c r="J541" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K541" s="1"/>
       <c r="L541" s="1">
@@ -33083,7 +33074,7 @@
         <v>153</v>
       </c>
       <c r="J542" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K542" s="6" t="s">
         <v>154</v>
@@ -33179,7 +33170,7 @@
         <v>174</v>
       </c>
       <c r="J544" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K544" s="1"/>
       <c r="L544" s="1">
@@ -33225,7 +33216,7 @@
         <v>174</v>
       </c>
       <c r="J545" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K545" s="1"/>
       <c r="L545" s="1">
@@ -33271,10 +33262,10 @@
         <v>147</v>
       </c>
       <c r="J546" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K546" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L546" s="5" t="s">
         <v>148</v>
@@ -33364,10 +33355,10 @@
         <v>688</v>
       </c>
       <c r="J548" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K548" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L548" s="5" t="s">
         <v>689</v>
@@ -33385,7 +33376,7 @@
     </row>
     <row r="549" spans="1:16">
       <c r="A549" s="17" t="s">
-        <v>1545</v>
+        <v>1542</v>
       </c>
       <c r="C549" s="7" t="s">
         <v>1450</v>
@@ -33409,10 +33400,10 @@
         <v>265</v>
       </c>
       <c r="J549" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K549" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L549" s="5" t="s">
         <v>266</v>
@@ -33505,7 +33496,7 @@
         <v>174</v>
       </c>
       <c r="J551" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K551" s="1"/>
       <c r="L551" s="1">
@@ -33551,7 +33542,7 @@
         <v>174</v>
       </c>
       <c r="J552" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K552" s="1"/>
       <c r="L552" s="1">
@@ -33645,10 +33636,10 @@
         <v>1090</v>
       </c>
       <c r="J554" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K554" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L554" s="5" t="s">
         <v>1091</v>
@@ -33693,10 +33684,10 @@
         <v>1090</v>
       </c>
       <c r="J555" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K555" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L555" s="5" t="s">
         <v>1091</v>
@@ -33714,7 +33705,7 @@
     </row>
     <row r="556" spans="1:16" ht="16" customHeight="1">
       <c r="A556" s="11" t="s">
-        <v>1546</v>
+        <v>1543</v>
       </c>
       <c r="B556" s="11" t="s">
         <v>887</v>
@@ -33885,10 +33876,10 @@
         <v>147</v>
       </c>
       <c r="J559" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K559" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L559" s="5" t="s">
         <v>148</v>
@@ -34125,7 +34116,7 @@
         <v>153</v>
       </c>
       <c r="J564" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K564" s="6" t="s">
         <v>154</v>
@@ -34221,10 +34212,10 @@
         <v>1382</v>
       </c>
       <c r="J566" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K566" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L566" s="5" t="s">
         <v>1411</v>
@@ -34317,10 +34308,10 @@
         <v>1090</v>
       </c>
       <c r="J568" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K568" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L568" s="5" t="s">
         <v>1091</v>
@@ -34386,7 +34377,7 @@
     </row>
     <row r="570" spans="1:16" ht="31">
       <c r="A570" s="24" t="s">
-        <v>1547</v>
+        <v>1544</v>
       </c>
       <c r="C570" s="29" t="s">
         <v>1450</v>
@@ -34407,10 +34398,10 @@
         <v>1086</v>
       </c>
       <c r="J570" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K570" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L570" s="5" t="s">
         <v>1087</v>
@@ -34425,12 +34416,12 @@
         <v>452</v>
       </c>
       <c r="P570" s="8" t="s">
-        <v>1548</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="571" spans="1:16" ht="31">
       <c r="A571" s="24" t="s">
-        <v>1547</v>
+        <v>1544</v>
       </c>
       <c r="C571" s="29" t="s">
         <v>1450</v>
@@ -34451,10 +34442,10 @@
         <v>1086</v>
       </c>
       <c r="J571" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K571" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L571" s="5" t="s">
         <v>1087</v>
@@ -34469,7 +34460,7 @@
         <v>452</v>
       </c>
       <c r="P571" s="8" t="s">
-        <v>1548</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="572" spans="1:16" ht="31">
@@ -34597,7 +34588,7 @@
         <v>174</v>
       </c>
       <c r="J574" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K574" s="1"/>
       <c r="L574" s="1">
@@ -34739,10 +34730,10 @@
         <v>1382</v>
       </c>
       <c r="J577" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K577" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L577" s="5" t="s">
         <v>1423</v>
@@ -35075,10 +35066,10 @@
         <v>1090</v>
       </c>
       <c r="J584" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K584" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L584" s="5" t="s">
         <v>1091</v>
@@ -35270,7 +35261,7 @@
         <v>72</v>
       </c>
       <c r="K588" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L588" s="5" t="s">
         <v>49</v>
@@ -35318,7 +35309,7 @@
         <v>72</v>
       </c>
       <c r="K589" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L589" s="5" t="s">
         <v>49</v>
@@ -35366,7 +35357,7 @@
         <v>72</v>
       </c>
       <c r="K590" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L590" s="5" t="s">
         <v>55</v>
@@ -35411,10 +35402,10 @@
         <v>147</v>
       </c>
       <c r="J591" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K591" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L591" s="5" t="s">
         <v>148</v>
@@ -35651,7 +35642,7 @@
         <v>153</v>
       </c>
       <c r="J596" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K596" s="6" t="s">
         <v>154</v>
@@ -35741,10 +35732,10 @@
         <v>688</v>
       </c>
       <c r="J598" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K598" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L598" s="5" t="s">
         <v>689</v>
@@ -35762,7 +35753,7 @@
     </row>
     <row r="599" spans="1:16" ht="31">
       <c r="A599" s="11" t="s">
-        <v>1549</v>
+        <v>1546</v>
       </c>
       <c r="B599" s="11" t="s">
         <v>901</v>
@@ -35933,10 +35924,10 @@
         <v>1382</v>
       </c>
       <c r="J602" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K602" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L602" s="5" t="s">
         <v>1422</v>
@@ -35984,7 +35975,7 @@
         <v>72</v>
       </c>
       <c r="K603" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L603" s="5" t="s">
         <v>49</v>
@@ -36029,7 +36020,7 @@
         <v>153</v>
       </c>
       <c r="J604" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K604" s="6" t="s">
         <v>154</v>
@@ -36077,7 +36068,7 @@
         <v>174</v>
       </c>
       <c r="J605" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K605" s="1"/>
       <c r="L605" s="1">
@@ -36123,7 +36114,7 @@
         <v>174</v>
       </c>
       <c r="J606" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K606" s="1"/>
       <c r="L606" s="1">
@@ -36679,7 +36670,7 @@
         <v>153</v>
       </c>
       <c r="J618" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K618" s="6" t="s">
         <v>154</v>
@@ -37015,10 +37006,10 @@
         <v>1382</v>
       </c>
       <c r="J625" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K625" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L625" s="5" t="s">
         <v>1436</v>
@@ -37237,10 +37228,10 @@
         <v>1086</v>
       </c>
       <c r="J630" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K630" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L630" s="5" t="s">
         <v>1087</v>
@@ -37285,7 +37276,7 @@
         <v>174</v>
       </c>
       <c r="J631" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K631" s="1"/>
       <c r="L631" s="1">
@@ -37331,7 +37322,7 @@
         <v>174</v>
       </c>
       <c r="J632" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K632" s="1"/>
       <c r="L632" s="1">
@@ -37377,7 +37368,7 @@
         <v>174</v>
       </c>
       <c r="J633" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K633" s="1"/>
       <c r="L633" s="1">
@@ -37526,7 +37517,7 @@
         <v>452</v>
       </c>
       <c r="P636" s="8" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="637" spans="1:16">
@@ -37558,10 +37549,10 @@
         <v>1090</v>
       </c>
       <c r="J637" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K637" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L637" s="5" t="s">
         <v>1091</v>
@@ -37651,10 +37642,10 @@
         <v>1090</v>
       </c>
       <c r="J639" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K639" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L639" s="5" t="s">
         <v>1091</v>
@@ -37891,10 +37882,10 @@
         <v>1382</v>
       </c>
       <c r="J644" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K644" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L644" s="5" t="s">
         <v>1433</v>
@@ -38269,10 +38260,10 @@
         <v>1086</v>
       </c>
       <c r="J652" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K652" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L652" s="5" t="s">
         <v>1087</v>
@@ -38557,10 +38548,10 @@
         <v>147</v>
       </c>
       <c r="J658" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K658" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L658" s="5" t="s">
         <v>148</v>
@@ -38845,10 +38836,10 @@
         <v>265</v>
       </c>
       <c r="J664" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K664" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L664" s="5" t="s">
         <v>266</v>
@@ -38930,10 +38921,10 @@
         <v>265</v>
       </c>
       <c r="J666" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K666" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L666" s="5" t="s">
         <v>266</v>
@@ -39065,10 +39056,10 @@
         <v>688</v>
       </c>
       <c r="J669" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K669" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L669" s="5" t="s">
         <v>689</v>
@@ -39113,10 +39104,10 @@
         <v>1382</v>
       </c>
       <c r="J670" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K670" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L670" s="5" t="s">
         <v>1429</v>
@@ -39161,10 +39152,10 @@
         <v>147</v>
       </c>
       <c r="J671" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K671" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L671" s="5" t="s">
         <v>148</v>
@@ -39545,10 +39536,10 @@
         <v>1382</v>
       </c>
       <c r="J679" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K679" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L679" s="5" t="s">
         <v>1430</v>
@@ -39737,7 +39728,7 @@
         <v>174</v>
       </c>
       <c r="J683" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K683" s="1"/>
       <c r="L683" s="1">
@@ -39783,10 +39774,10 @@
         <v>1090</v>
       </c>
       <c r="J684" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K684" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L684" s="5" t="s">
         <v>1091</v>
@@ -39930,7 +39921,7 @@
         <v>72</v>
       </c>
       <c r="K687" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L687" s="5" t="s">
         <v>49</v>
@@ -39975,7 +39966,7 @@
         <v>72</v>
       </c>
       <c r="K688" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L688" s="5" t="s">
         <v>56</v>
@@ -40116,10 +40107,10 @@
         <v>147</v>
       </c>
       <c r="J691" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K691" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L691" s="5" t="s">
         <v>148</v>
@@ -40206,10 +40197,10 @@
         <v>1181</v>
       </c>
       <c r="J693" s="23" t="s">
-        <v>1597</v>
+        <v>1594</v>
       </c>
       <c r="K693" s="6" t="s">
-        <v>1598</v>
+        <v>1595</v>
       </c>
       <c r="L693" s="5" t="s">
         <v>1182</v>
@@ -40227,7 +40218,7 @@
     </row>
     <row r="694" spans="1:16">
       <c r="A694" s="2" t="s">
-        <v>1551</v>
+        <v>1548</v>
       </c>
       <c r="B694" s="19" t="s">
         <v>736</v>
@@ -40302,10 +40293,10 @@
         <v>147</v>
       </c>
       <c r="J695" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K695" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L695" s="5" t="s">
         <v>148</v>
@@ -40392,10 +40383,10 @@
         <v>1086</v>
       </c>
       <c r="J697" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K697" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L697" s="5" t="s">
         <v>1087</v>
@@ -40440,10 +40431,10 @@
         <v>123</v>
       </c>
       <c r="J698" s="6" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="K698" s="6" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
       <c r="L698" s="5" t="s">
         <v>124</v>
@@ -40488,10 +40479,10 @@
         <v>123</v>
       </c>
       <c r="J699" s="6" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="K699" s="6" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
       <c r="L699" s="5" t="s">
         <v>124</v>
@@ -40536,10 +40527,10 @@
         <v>123</v>
       </c>
       <c r="J700" s="6" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="K700" s="6" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
       <c r="L700" s="5" t="s">
         <v>124</v>
@@ -40584,10 +40575,10 @@
         <v>123</v>
       </c>
       <c r="J701" s="6" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="K701" s="6" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
       <c r="L701" s="5" t="s">
         <v>124</v>
@@ -40632,10 +40623,10 @@
         <v>265</v>
       </c>
       <c r="J702" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K702" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L702" s="5" t="s">
         <v>266</v>
@@ -40728,10 +40719,10 @@
         <v>147</v>
       </c>
       <c r="J704" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K704" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L704" s="5" t="s">
         <v>148</v>
@@ -41160,7 +41151,7 @@
         <v>72</v>
       </c>
       <c r="K713" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L713" s="5" t="s">
         <v>49</v>
@@ -41253,7 +41244,7 @@
         <v>153</v>
       </c>
       <c r="J715" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K715" s="6" t="s">
         <v>154</v>
@@ -41349,10 +41340,10 @@
         <v>147</v>
       </c>
       <c r="J717" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K717" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L717" s="5" t="s">
         <v>148</v>
@@ -41397,7 +41388,7 @@
         <v>174</v>
       </c>
       <c r="J718" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K718" s="1"/>
       <c r="L718" s="1">
@@ -41443,7 +41434,7 @@
         <v>174</v>
       </c>
       <c r="J719" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K719" s="1"/>
       <c r="L719" s="1">
@@ -41489,7 +41480,7 @@
         <v>174</v>
       </c>
       <c r="J720" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K720" s="1"/>
       <c r="L720" s="1">
@@ -41721,10 +41712,10 @@
         <v>1086</v>
       </c>
       <c r="J725" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K725" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L725" s="5" t="s">
         <v>1087</v>
@@ -41814,10 +41805,10 @@
         <v>147</v>
       </c>
       <c r="J727" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K727" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L727" s="5" t="s">
         <v>148</v>
@@ -42054,10 +42045,10 @@
         <v>1382</v>
       </c>
       <c r="J732" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K732" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L732" s="5" t="s">
         <v>1431</v>
@@ -42105,7 +42096,7 @@
         <v>72</v>
       </c>
       <c r="K733" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L733" s="5" t="s">
         <v>49</v>
@@ -42216,7 +42207,7 @@
     </row>
     <row r="736" spans="1:16">
       <c r="A736" s="19" t="s">
-        <v>1552</v>
+        <v>1549</v>
       </c>
       <c r="B736" s="27" t="s">
         <v>794</v>
@@ -42264,7 +42255,7 @@
     </row>
     <row r="737" spans="1:16">
       <c r="A737" s="2" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="B737" s="2" t="s">
         <v>448</v>
@@ -42312,7 +42303,7 @@
     </row>
     <row r="738" spans="1:16">
       <c r="A738" s="2" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="B738" s="2" t="s">
         <v>448</v>
@@ -42360,7 +42351,7 @@
     </row>
     <row r="739" spans="1:16">
       <c r="A739" s="2" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="B739" s="2" t="s">
         <v>448</v>
@@ -42408,7 +42399,7 @@
     </row>
     <row r="740" spans="1:16">
       <c r="A740" s="2" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="B740" s="2" t="s">
         <v>448</v>
@@ -42531,10 +42522,10 @@
         <v>1090</v>
       </c>
       <c r="J742" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K742" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L742" s="5" t="s">
         <v>1091</v>
@@ -42579,10 +42570,10 @@
         <v>691</v>
       </c>
       <c r="J743" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K743" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L743" s="5" t="s">
         <v>692</v>
@@ -42768,10 +42759,10 @@
         <v>1382</v>
       </c>
       <c r="J747" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K747" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L747" s="5" t="s">
         <v>1424</v>
@@ -42861,7 +42852,7 @@
         <v>174</v>
       </c>
       <c r="J749" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K749" s="1"/>
       <c r="L749" s="1">
@@ -43195,10 +43186,10 @@
         <v>265</v>
       </c>
       <c r="J756" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K756" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L756" s="5" t="s">
         <v>266</v>
@@ -43700,10 +43691,10 @@
         <v>688</v>
       </c>
       <c r="J767" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K767" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L767" s="5" t="s">
         <v>689</v>
@@ -43769,7 +43760,7 @@
     </row>
     <row r="769" spans="1:16">
       <c r="A769" s="2" t="s">
-        <v>1554</v>
+        <v>1551</v>
       </c>
       <c r="C769" s="29" t="s">
         <v>1449</v>
@@ -43833,7 +43824,7 @@
         <v>174</v>
       </c>
       <c r="J770" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K770" s="1"/>
       <c r="L770" s="1">
@@ -44119,10 +44110,10 @@
         <v>147</v>
       </c>
       <c r="J776" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K776" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L776" s="5" t="s">
         <v>148</v>
@@ -44263,7 +44254,7 @@
         <v>174</v>
       </c>
       <c r="J779" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K779" s="1"/>
       <c r="L779" s="1">
@@ -44291,7 +44282,7 @@
         <v>1450</v>
       </c>
       <c r="D780" s="7" t="s">
-        <v>1602</v>
+        <v>1599</v>
       </c>
       <c r="E780" s="1" t="s">
         <v>1134</v>
@@ -44312,7 +44303,7 @@
         <v>72</v>
       </c>
       <c r="K780" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L780" s="5" t="s">
         <v>49</v>
@@ -44444,10 +44435,10 @@
         <v>1086</v>
       </c>
       <c r="J783" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K783" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L783" s="5" t="s">
         <v>1087</v>
@@ -44588,10 +44579,10 @@
         <v>265</v>
       </c>
       <c r="J786" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K786" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L786" s="5" t="s">
         <v>266</v>
@@ -44771,7 +44762,7 @@
         <v>174</v>
       </c>
       <c r="J790" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K790" s="1"/>
       <c r="L790" s="1">
@@ -44817,7 +44808,7 @@
         <v>174</v>
       </c>
       <c r="J791" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K791" s="1"/>
       <c r="L791" s="1">
@@ -44911,10 +44902,10 @@
         <v>147</v>
       </c>
       <c r="J793" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K793" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L793" s="5" t="s">
         <v>148</v>
@@ -45196,10 +45187,10 @@
         <v>688</v>
       </c>
       <c r="J799" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K799" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L799" s="5" t="s">
         <v>689</v>
@@ -45265,7 +45256,7 @@
     </row>
     <row r="801" spans="1:16">
       <c r="A801" s="19" t="s">
-        <v>1555</v>
+        <v>1552</v>
       </c>
       <c r="B801" s="19" t="s">
         <v>769</v>
@@ -45334,10 +45325,10 @@
         <v>1181</v>
       </c>
       <c r="J802" s="23" t="s">
-        <v>1597</v>
+        <v>1594</v>
       </c>
       <c r="K802" s="6" t="s">
-        <v>1598</v>
+        <v>1595</v>
       </c>
       <c r="L802" s="5" t="s">
         <v>1182</v>
@@ -45499,7 +45490,7 @@
         <v>397</v>
       </c>
       <c r="B806" s="2" t="s">
-        <v>1557</v>
+        <v>1554</v>
       </c>
       <c r="C806" s="29" t="s">
         <v>1450</v>
@@ -45523,7 +45514,7 @@
         <v>174</v>
       </c>
       <c r="J806" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K806" s="1"/>
       <c r="L806" s="1">
@@ -45641,7 +45632,7 @@
         <v>397</v>
       </c>
       <c r="B809" s="24" t="s">
-        <v>1556</v>
+        <v>1553</v>
       </c>
       <c r="C809" s="1" t="s">
         <v>1450</v>
@@ -45854,7 +45845,7 @@
         <v>72</v>
       </c>
       <c r="K813" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L813" s="5" t="s">
         <v>49</v>
@@ -45869,7 +45860,7 @@
         <v>452</v>
       </c>
       <c r="P813" s="21" t="s">
-        <v>1603</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="814" spans="1:16">
@@ -45997,10 +45988,10 @@
         <v>1382</v>
       </c>
       <c r="J816" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K816" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L816" s="5" t="s">
         <v>1425</v>
@@ -46015,7 +46006,7 @@
         <v>452</v>
       </c>
       <c r="P816" s="47" t="s">
-        <v>1604</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="817" spans="1:16">
@@ -46050,7 +46041,7 @@
         <v>72</v>
       </c>
       <c r="K817" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L817" s="5" t="s">
         <v>49</v>
@@ -46095,10 +46086,10 @@
         <v>147</v>
       </c>
       <c r="J818" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K818" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L818" s="5" t="s">
         <v>148</v>
@@ -46278,7 +46269,7 @@
         <v>174</v>
       </c>
       <c r="J822" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K822" s="1"/>
       <c r="L822" s="1">
@@ -46468,7 +46459,7 @@
         <v>153</v>
       </c>
       <c r="J826" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K826" s="6" t="s">
         <v>154</v>
@@ -46846,10 +46837,10 @@
         <v>688</v>
       </c>
       <c r="J834" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K834" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L834" s="5" t="s">
         <v>689</v>
@@ -46870,7 +46861,7 @@
         <v>6</v>
       </c>
       <c r="B835" s="2" t="s">
-        <v>1558</v>
+        <v>1555</v>
       </c>
       <c r="C835" s="7" t="s">
         <v>1450</v>
@@ -46894,10 +46885,10 @@
         <v>265</v>
       </c>
       <c r="J835" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K835" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L835" s="5" t="s">
         <v>266</v>
@@ -46912,7 +46903,7 @@
         <v>452</v>
       </c>
       <c r="P835" s="47" t="s">
-        <v>1605</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="836" spans="1:16">
@@ -46944,10 +46935,10 @@
         <v>265</v>
       </c>
       <c r="J836" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K836" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L836" s="5" t="s">
         <v>266</v>
@@ -46968,7 +46959,7 @@
         <v>580</v>
       </c>
       <c r="B837" s="2" t="s">
-        <v>1559</v>
+        <v>1556</v>
       </c>
       <c r="C837" s="29" t="s">
         <v>1450</v>
@@ -46992,10 +46983,10 @@
         <v>1090</v>
       </c>
       <c r="J837" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K837" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L837" s="5" t="s">
         <v>1091</v>
@@ -47010,7 +47001,7 @@
         <v>452</v>
       </c>
       <c r="P837" s="8" t="s">
-        <v>1606</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="838" spans="1:16">
@@ -47186,10 +47177,10 @@
         <v>1382</v>
       </c>
       <c r="J841" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K841" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L841" s="5" t="s">
         <v>1426</v>
@@ -47426,10 +47417,10 @@
         <v>1382</v>
       </c>
       <c r="J846" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K846" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L846" s="5" t="s">
         <v>1427</v>
@@ -47522,10 +47513,10 @@
         <v>147</v>
       </c>
       <c r="J848" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K848" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L848" s="5" t="s">
         <v>148</v>
@@ -47618,7 +47609,7 @@
         <v>153</v>
       </c>
       <c r="J850" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K850" s="6" t="s">
         <v>154</v>
@@ -47714,7 +47705,7 @@
         <v>153</v>
       </c>
       <c r="J852" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K852" s="6" t="s">
         <v>154</v>
@@ -47810,10 +47801,10 @@
         <v>1090</v>
       </c>
       <c r="J854" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K854" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L854" s="5" t="s">
         <v>1091</v>
@@ -47831,7 +47822,7 @@
     </row>
     <row r="855" spans="1:16">
       <c r="A855" s="19" t="s">
-        <v>1560</v>
+        <v>1557</v>
       </c>
       <c r="B855" s="19" t="s">
         <v>770</v>
@@ -47879,7 +47870,7 @@
     </row>
     <row r="856" spans="1:16">
       <c r="A856" s="19" t="s">
-        <v>1561</v>
+        <v>1558</v>
       </c>
       <c r="B856" s="19" t="s">
         <v>771</v>
@@ -47927,7 +47918,7 @@
     </row>
     <row r="857" spans="1:16" ht="31">
       <c r="A857" s="24" t="s">
-        <v>1562</v>
+        <v>1559</v>
       </c>
       <c r="B857" s="11" t="s">
         <v>884</v>
@@ -48092,10 +48083,10 @@
         <v>1086</v>
       </c>
       <c r="J860" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K860" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L860" s="5" t="s">
         <v>1087</v>
@@ -48284,7 +48275,7 @@
         <v>174</v>
       </c>
       <c r="J864" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K864" s="1"/>
       <c r="L864" s="1">
@@ -48378,10 +48369,10 @@
         <v>691</v>
       </c>
       <c r="J866" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K866" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L866" s="5" t="s">
         <v>692</v>
@@ -48525,7 +48516,7 @@
         <v>72</v>
       </c>
       <c r="K869" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L869" s="5" t="s">
         <v>49</v>
@@ -48945,10 +48936,10 @@
         <v>1382</v>
       </c>
       <c r="J878" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K878" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L878" s="5" t="s">
         <v>1418</v>
@@ -49035,10 +49026,10 @@
         <v>1086</v>
       </c>
       <c r="J880" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K880" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L880" s="5" t="s">
         <v>1087</v>
@@ -49083,7 +49074,7 @@
         <v>174</v>
       </c>
       <c r="J881" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K881" s="1"/>
       <c r="L881" s="1">
@@ -49129,7 +49120,7 @@
         <v>174</v>
       </c>
       <c r="J882" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K882" s="1"/>
       <c r="L882" s="1">
@@ -49220,10 +49211,10 @@
         <v>1090</v>
       </c>
       <c r="J884" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K884" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L884" s="5" t="s">
         <v>1091</v>
@@ -49316,10 +49307,10 @@
         <v>147</v>
       </c>
       <c r="J886" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K886" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L886" s="5" t="s">
         <v>148</v>
@@ -49739,10 +49730,10 @@
         <v>147</v>
       </c>
       <c r="J895" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K895" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L895" s="5" t="s">
         <v>148</v>
@@ -49763,7 +49754,7 @@
         <v>506</v>
       </c>
       <c r="B896" s="42" t="s">
-        <v>1563</v>
+        <v>1560</v>
       </c>
       <c r="C896" s="32" t="s">
         <v>1450</v>
@@ -49883,10 +49874,10 @@
         <v>147</v>
       </c>
       <c r="J898" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K898" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L898" s="5" t="s">
         <v>148</v>
@@ -49973,10 +49964,10 @@
         <v>688</v>
       </c>
       <c r="J900" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K900" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L900" s="5" t="s">
         <v>689</v>
@@ -50111,10 +50102,10 @@
         <v>1086</v>
       </c>
       <c r="J903" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K903" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L903" s="5" t="s">
         <v>1087</v>
@@ -50351,10 +50342,10 @@
         <v>147</v>
       </c>
       <c r="J908" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K908" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L908" s="5" t="s">
         <v>148</v>
@@ -50375,7 +50366,7 @@
         <v>847</v>
       </c>
       <c r="B909" s="24" t="s">
-        <v>1565</v>
+        <v>1562</v>
       </c>
       <c r="C909" s="1" t="s">
         <v>1450</v>
@@ -50420,7 +50411,7 @@
     </row>
     <row r="910" spans="1:16">
       <c r="A910" s="19" t="s">
-        <v>1564</v>
+        <v>1561</v>
       </c>
       <c r="B910" s="19" t="s">
         <v>751</v>
@@ -50498,7 +50489,7 @@
         <v>72</v>
       </c>
       <c r="K911" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L911" s="5" t="s">
         <v>49</v>
@@ -50516,7 +50507,7 @@
     </row>
     <row r="912" spans="1:16" ht="17.5" customHeight="1">
       <c r="A912" s="12" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="B912" s="12" t="s">
         <v>739</v>
@@ -50543,10 +50534,10 @@
         <v>1382</v>
       </c>
       <c r="J912" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K912" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L912" s="5" t="s">
         <v>1421</v>
@@ -50561,12 +50552,12 @@
         <v>452</v>
       </c>
       <c r="P912" s="8" t="s">
-        <v>1567</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="913" spans="1:16">
       <c r="A913" s="12" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="B913" s="19" t="s">
         <v>739</v>
@@ -50614,7 +50605,7 @@
     </row>
     <row r="914" spans="1:16" ht="18.5" customHeight="1">
       <c r="A914" s="12" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="B914" s="11" t="s">
         <v>739</v>
@@ -50665,7 +50656,7 @@
         <v>645</v>
       </c>
       <c r="B915" s="18" t="s">
-        <v>1566</v>
+        <v>1563</v>
       </c>
       <c r="C915" s="29" t="s">
         <v>1450</v>
@@ -50713,7 +50704,7 @@
         <v>645</v>
       </c>
       <c r="B916" s="18" t="s">
-        <v>1566</v>
+        <v>1563</v>
       </c>
       <c r="C916" s="29" t="s">
         <v>1450</v>
@@ -50779,10 +50770,10 @@
         <v>1086</v>
       </c>
       <c r="J917" s="23" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="K917" s="6" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="L917" s="5" t="s">
         <v>1087</v>
@@ -50923,10 +50914,10 @@
         <v>265</v>
       </c>
       <c r="J920" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K920" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L920" s="5" t="s">
         <v>266</v>
@@ -51067,7 +51058,7 @@
         <v>174</v>
       </c>
       <c r="J923" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K923" s="1"/>
       <c r="L923" s="1">
@@ -51089,7 +51080,7 @@
         <v>547</v>
       </c>
       <c r="B924" s="18" t="s">
-        <v>1569</v>
+        <v>1566</v>
       </c>
       <c r="C924" s="29" t="s">
         <v>1450</v>
@@ -51182,10 +51173,10 @@
     </row>
     <row r="926" spans="1:16">
       <c r="A926" s="42" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="B926" s="42" t="s">
-        <v>1571</v>
+        <v>1568</v>
       </c>
       <c r="C926" s="32" t="s">
         <v>1450</v>
@@ -51230,10 +51221,10 @@
     </row>
     <row r="927" spans="1:16">
       <c r="A927" s="42" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="B927" s="42" t="s">
-        <v>1571</v>
+        <v>1568</v>
       </c>
       <c r="C927" s="32" t="s">
         <v>1450</v>
@@ -51278,10 +51269,10 @@
     </row>
     <row r="928" spans="1:16">
       <c r="A928" s="42" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="B928" s="42" t="s">
-        <v>1571</v>
+        <v>1568</v>
       </c>
       <c r="C928" s="32" t="s">
         <v>1452</v>
@@ -51326,10 +51317,10 @@
     </row>
     <row r="929" spans="1:16">
       <c r="A929" s="42" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="B929" s="42" t="s">
-        <v>1571</v>
+        <v>1568</v>
       </c>
       <c r="C929" s="32" t="s">
         <v>1453</v>
@@ -51374,10 +51365,10 @@
     </row>
     <row r="930" spans="1:16">
       <c r="A930" s="42" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="B930" s="42" t="s">
-        <v>1571</v>
+        <v>1568</v>
       </c>
       <c r="C930" s="32" t="s">
         <v>1454</v>
@@ -51449,10 +51440,10 @@
         <v>1382</v>
       </c>
       <c r="J931" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K931" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L931" s="5" t="s">
         <v>1428</v>
@@ -51569,7 +51560,7 @@
         <v>754</v>
       </c>
       <c r="B934" s="49" t="s">
-        <v>1572</v>
+        <v>1569</v>
       </c>
       <c r="C934" s="29" t="s">
         <v>1450</v>
@@ -51611,7 +51602,7 @@
         <v>452</v>
       </c>
       <c r="P934" s="48" t="s">
-        <v>1607</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="935" spans="1:16">
@@ -51787,10 +51778,10 @@
         <v>1382</v>
       </c>
       <c r="J938" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K938" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L938" s="5" t="s">
         <v>1437</v>
@@ -51989,7 +51980,7 @@
     </row>
     <row r="943" spans="1:16">
       <c r="A943" s="19" t="s">
-        <v>1573</v>
+        <v>1570</v>
       </c>
       <c r="B943" s="19" t="s">
         <v>735</v>
@@ -52685,7 +52676,7 @@
         <v>174</v>
       </c>
       <c r="J957" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K957" s="1"/>
       <c r="L957" s="1">
@@ -52851,7 +52842,7 @@
         <v>46</v>
       </c>
       <c r="B961" s="2" t="s">
-        <v>1574</v>
+        <v>1571</v>
       </c>
       <c r="C961" s="29" t="s">
         <v>1450</v>
@@ -52893,7 +52884,7 @@
         <v>452</v>
       </c>
       <c r="P961" s="8" t="s">
-        <v>1575</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="962" spans="1:16">
@@ -52925,10 +52916,10 @@
         <v>147</v>
       </c>
       <c r="J962" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K962" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L962" s="5" t="s">
         <v>148</v>
@@ -52973,10 +52964,10 @@
         <v>1382</v>
       </c>
       <c r="J963" s="6" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="K963" s="6" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="L963" s="5" t="s">
         <v>1417</v>
@@ -53024,7 +53015,7 @@
         <v>72</v>
       </c>
       <c r="K964" s="6" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="L964" s="5" t="s">
         <v>49</v>
@@ -53213,7 +53204,7 @@
         <v>153</v>
       </c>
       <c r="J968" s="6" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="K968" s="6" t="s">
         <v>154</v>
@@ -53261,7 +53252,7 @@
         <v>174</v>
       </c>
       <c r="J969" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K969" s="1"/>
       <c r="L969" s="1">
@@ -53283,7 +53274,7 @@
         <v>46</v>
       </c>
       <c r="B970" s="42" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
       <c r="C970" s="32" t="s">
         <v>1450</v>
@@ -53400,10 +53391,10 @@
         <v>1090</v>
       </c>
       <c r="J972" s="23" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="K972" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="L972" s="5" t="s">
         <v>1091</v>
@@ -53448,7 +53439,7 @@
         <v>174</v>
       </c>
       <c r="J973" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="K973" s="1"/>
       <c r="L973" s="1">
@@ -53590,10 +53581,10 @@
         <v>265</v>
       </c>
       <c r="J976" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K976" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L976" s="5" t="s">
         <v>266</v>
@@ -53614,7 +53605,7 @@
         <v>396</v>
       </c>
       <c r="B977" s="42" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="C977" s="32" t="s">
         <v>1450</v>
@@ -53662,7 +53653,7 @@
         <v>396</v>
       </c>
       <c r="B978" s="42" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="C978" s="32" t="s">
         <v>1451</v>
@@ -53710,7 +53701,7 @@
         <v>396</v>
       </c>
       <c r="B979" s="42" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="C979" s="32" t="s">
         <v>1449</v>
@@ -53758,7 +53749,7 @@
         <v>396</v>
       </c>
       <c r="B980" s="42" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="C980" s="32" t="s">
         <v>1452</v>
@@ -53806,7 +53797,7 @@
         <v>396</v>
       </c>
       <c r="B981" s="42" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="C981" s="32" t="s">
         <v>1454</v>
@@ -53854,7 +53845,7 @@
         <v>396</v>
       </c>
       <c r="B982" s="42" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="C982" s="32" t="s">
         <v>1453</v>
@@ -53902,7 +53893,7 @@
         <v>396</v>
       </c>
       <c r="B983" s="42" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="C983" s="32" t="s">
         <v>1455</v>
@@ -54106,10 +54097,10 @@
         <v>688</v>
       </c>
       <c r="J987" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K987" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L987" s="5" t="s">
         <v>689</v>
@@ -54151,10 +54142,10 @@
         <v>688</v>
       </c>
       <c r="J988" s="6" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="K988" s="6" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="L988" s="5" t="s">
         <v>689</v>
@@ -54428,10 +54419,10 @@
         <v>265</v>
       </c>
       <c r="J994" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K994" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L994" s="5" t="s">
         <v>266</v>
@@ -54476,10 +54467,10 @@
         <v>265</v>
       </c>
       <c r="J995" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K995" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L995" s="5" t="s">
         <v>266</v>
@@ -54620,10 +54611,10 @@
         <v>147</v>
       </c>
       <c r="J998" s="6" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="K998" s="6" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="L998" s="5" t="s">
         <v>148</v>
@@ -55327,7 +55318,7 @@
         <v>174</v>
       </c>
       <c r="J1013" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="L1013" s="1">
         <v>2017</v>
@@ -55371,7 +55362,7 @@
         <v>174</v>
       </c>
       <c r="J1014" s="23" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="L1014" s="1">
         <v>2017</v>
@@ -55579,7 +55570,7 @@
         <v>393</v>
       </c>
       <c r="B1019" s="42" t="s">
-        <v>1578</v>
+        <v>1575</v>
       </c>
       <c r="C1019" s="32" t="s">
         <v>1455</v>
@@ -56022,10 +56013,10 @@
         <v>265</v>
       </c>
       <c r="J1028" s="6" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="K1028" s="6" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="L1028" s="5" t="s">
         <v>266</v>
@@ -56116,10 +56107,10 @@
         <v>691</v>
       </c>
       <c r="J1030" s="23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="K1030" s="6" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="L1030" s="5" t="s">
         <v>692</v>
@@ -56186,21 +56177,12 @@
       <c r="I1032" s="5"/>
     </row>
     <row r="1033" spans="1:15">
-      <c r="D1033" s="1" t="s">
-        <v>1502</v>
-      </c>
       <c r="I1033" s="5"/>
     </row>
     <row r="1034" spans="1:15">
-      <c r="D1034" s="1" t="s">
-        <v>1503</v>
-      </c>
       <c r="I1034" s="5"/>
     </row>
     <row r="1035" spans="1:15">
-      <c r="D1035" s="1" t="s">
-        <v>1504</v>
-      </c>
       <c r="I1035" s="5"/>
     </row>
     <row r="1036" spans="1:15">

</xml_diff>